<commit_message>
Aggiornato data.json con il caso id 39; Aggiornato il report; Caricato il PDF per il caso id 39;
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111GESAN000000/GESAN_SRL/WLEXT-RIS/V.2.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111GESAN000000/GESAN_SRL/WLEXT-RIS/V.2.0/report-checklist.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="171">
   <si>
     <t>NOME FORNITORE:</t>
   </si>
@@ -307,6 +307,9 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.150.4.4.94acb62a90ecf2b5970963e2b6ccecc38052be0abcb8d84f43ef841412b8d449.32cf0b5124^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>JWT payload: Person id presente nel JWT differente dal codice fiscale del paziente previsto sul CDA</t>
   </si>
   <si>
     <t>L’applicativo risponde con un codice di errore e il messaggio “Campo token JWT non valido” seguito dal motivo dell’errore. Il referto non viene prodotto</t>
@@ -3124,12 +3127,20 @@
         <v>31</v>
       </c>
       <c r="K15" s="50"/>
-      <c r="L15" s="39"/>
-      <c r="M15" s="39"/>
-      <c r="N15" s="38"/>
-      <c r="O15" s="39"/>
+      <c r="L15" t="s" s="37">
+        <v>31</v>
+      </c>
+      <c r="M15" t="s" s="37">
+        <v>47</v>
+      </c>
+      <c r="N15" t="s" s="47">
+        <v>55</v>
+      </c>
+      <c r="O15" t="s" s="37">
+        <v>31</v>
+      </c>
       <c r="P15" t="s" s="47">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="Q15" s="39"/>
       <c r="R15" s="37"/>
@@ -3149,16 +3160,16 @@
         <v>26</v>
       </c>
       <c r="D16" t="s" s="31">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E16" t="s" s="32">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F16" s="51">
         <v>44987</v>
       </c>
       <c r="G16" t="s" s="49">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H16" s="52"/>
       <c r="I16" s="52"/>
@@ -3166,10 +3177,10 @@
       <c r="K16" s="38"/>
       <c r="L16" s="39"/>
       <c r="M16" s="39"/>
-      <c r="N16" s="38"/>
+      <c r="N16" s="50"/>
       <c r="O16" s="39"/>
       <c r="P16" t="s" s="53">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="Q16" s="39"/>
       <c r="R16" t="s" s="37">
@@ -3191,10 +3202,10 @@
         <v>26</v>
       </c>
       <c r="D17" t="s" s="31">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E17" t="s" s="54">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="F17" s="55"/>
       <c r="G17" s="55"/>
@@ -3204,7 +3215,7 @@
         <v>47</v>
       </c>
       <c r="K17" t="s" s="37">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="L17" s="39"/>
       <c r="M17" s="39"/>
@@ -3229,10 +3240,10 @@
         <v>26</v>
       </c>
       <c r="D18" t="s" s="31">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E18" t="s" s="32">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F18" s="33"/>
       <c r="G18" s="33"/>
@@ -3242,7 +3253,7 @@
         <v>47</v>
       </c>
       <c r="K18" t="s" s="37">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="L18" s="39"/>
       <c r="M18" s="39"/>
@@ -3267,10 +3278,10 @@
         <v>26</v>
       </c>
       <c r="D19" t="s" s="31">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E19" t="s" s="32">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F19" s="33">
         <v>44981</v>
@@ -3279,10 +3290,10 @@
         <v>1.611111111111111</v>
       </c>
       <c r="H19" t="s" s="35">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I19" t="s" s="36">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="J19" t="s" s="37">
         <v>31</v>
@@ -3295,13 +3306,13 @@
         <v>47</v>
       </c>
       <c r="N19" t="s" s="36">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="O19" t="s" s="37">
         <v>31</v>
       </c>
       <c r="P19" t="s" s="37">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="Q19" s="39"/>
       <c r="R19" s="37"/>
@@ -3321,10 +3332,10 @@
         <v>26</v>
       </c>
       <c r="D20" t="s" s="31">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E20" t="s" s="32">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F20" s="33">
         <v>44981</v>
@@ -3333,10 +3344,10 @@
         <v>1.6125</v>
       </c>
       <c r="H20" t="s" s="44">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="I20" t="s" s="45">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="J20" t="s" s="37">
         <v>31</v>
@@ -3349,13 +3360,13 @@
         <v>31</v>
       </c>
       <c r="N20" t="s" s="45">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="O20" t="s" s="37">
         <v>47</v>
       </c>
       <c r="P20" t="s" s="37">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="Q20" s="39"/>
       <c r="R20" s="37"/>
@@ -3375,10 +3386,10 @@
         <v>26</v>
       </c>
       <c r="D21" t="s" s="31">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E21" t="s" s="32">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F21" s="33"/>
       <c r="G21" s="33"/>
@@ -3388,7 +3399,7 @@
         <v>47</v>
       </c>
       <c r="K21" t="s" s="37">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="L21" s="39"/>
       <c r="M21" s="39"/>
@@ -3413,10 +3424,10 @@
         <v>26</v>
       </c>
       <c r="D22" t="s" s="31">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E22" t="s" s="32">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F22" s="33"/>
       <c r="G22" s="33"/>
@@ -3426,7 +3437,7 @@
         <v>47</v>
       </c>
       <c r="K22" t="s" s="37">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="L22" s="39"/>
       <c r="M22" s="39"/>
@@ -3451,10 +3462,10 @@
         <v>26</v>
       </c>
       <c r="D23" t="s" s="31">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="E23" t="s" s="32">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F23" s="33">
         <v>44981</v>
@@ -3463,10 +3474,10 @@
         <v>1.665277777777778</v>
       </c>
       <c r="H23" t="s" s="59">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="I23" t="s" s="60">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="J23" t="s" s="37">
         <v>31</v>
@@ -3479,13 +3490,13 @@
         <v>31</v>
       </c>
       <c r="N23" t="s" s="60">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="O23" t="s" s="37">
         <v>47</v>
       </c>
       <c r="P23" t="s" s="37">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="Q23" s="39"/>
       <c r="R23" s="37"/>
@@ -3505,10 +3516,10 @@
         <v>26</v>
       </c>
       <c r="D24" t="s" s="31">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E24" t="s" s="32">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F24" s="33"/>
       <c r="G24" s="33"/>
@@ -3518,7 +3529,7 @@
         <v>47</v>
       </c>
       <c r="K24" t="s" s="37">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="L24" s="39"/>
       <c r="M24" s="39"/>
@@ -3543,10 +3554,10 @@
         <v>26</v>
       </c>
       <c r="D25" t="s" s="31">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E25" t="s" s="32">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="F25" s="33"/>
       <c r="G25" s="33"/>
@@ -3556,7 +3567,7 @@
         <v>47</v>
       </c>
       <c r="K25" t="s" s="37">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="L25" s="39"/>
       <c r="M25" s="39"/>
@@ -3581,10 +3592,10 @@
         <v>26</v>
       </c>
       <c r="D26" t="s" s="31">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E26" t="s" s="32">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F26" s="33">
         <v>44981</v>
@@ -3593,10 +3604,10 @@
         <v>1.613194444444444</v>
       </c>
       <c r="H26" t="s" s="59">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="I26" t="s" s="60">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="J26" t="s" s="37">
         <v>31</v>
@@ -3609,13 +3620,13 @@
         <v>31</v>
       </c>
       <c r="N26" t="s" s="60">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="O26" t="s" s="37">
         <v>47</v>
       </c>
       <c r="P26" t="s" s="37">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="Q26" s="39"/>
       <c r="R26" s="37"/>
@@ -3635,10 +3646,10 @@
         <v>26</v>
       </c>
       <c r="D27" t="s" s="31">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E27" t="s" s="32">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="F27" s="33"/>
       <c r="G27" s="33"/>
@@ -3648,7 +3659,7 @@
         <v>47</v>
       </c>
       <c r="K27" t="s" s="37">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="L27" s="39"/>
       <c r="M27" s="39"/>
@@ -3673,10 +3684,10 @@
         <v>26</v>
       </c>
       <c r="D28" t="s" s="31">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E28" t="s" s="32">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="F28" s="33">
         <v>44981</v>
@@ -3685,10 +3696,10 @@
         <v>1.609027777777778</v>
       </c>
       <c r="H28" t="s" s="35">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="I28" t="s" s="36">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="J28" t="s" s="37">
         <v>31</v>
@@ -3701,13 +3712,13 @@
         <v>31</v>
       </c>
       <c r="N28" t="s" s="36">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="O28" t="s" s="37">
         <v>47</v>
       </c>
       <c r="P28" t="s" s="37">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="Q28" s="39"/>
       <c r="R28" s="37"/>
@@ -3727,10 +3738,10 @@
         <v>26</v>
       </c>
       <c r="D29" t="s" s="31">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E29" t="s" s="32">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="F29" s="33">
         <v>44981</v>
@@ -3739,10 +3750,10 @@
         <v>1.634027777777778</v>
       </c>
       <c r="H29" t="s" s="42">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="I29" t="s" s="43">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="J29" t="s" s="37">
         <v>31</v>
@@ -3755,13 +3766,13 @@
         <v>31</v>
       </c>
       <c r="N29" t="s" s="43">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="O29" t="s" s="37">
         <v>47</v>
       </c>
       <c r="P29" t="s" s="37">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="Q29" s="39"/>
       <c r="R29" s="37"/>
@@ -3781,10 +3792,10 @@
         <v>26</v>
       </c>
       <c r="D30" t="s" s="31">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E30" t="s" s="32">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F30" s="33">
         <v>44984</v>
@@ -3793,10 +3804,10 @@
         <v>1.517361111111111</v>
       </c>
       <c r="H30" t="s" s="42">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="I30" t="s" s="43">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="J30" t="s" s="37">
         <v>31</v>
@@ -3809,13 +3820,13 @@
         <v>31</v>
       </c>
       <c r="N30" t="s" s="43">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="O30" t="s" s="37">
         <v>47</v>
       </c>
       <c r="P30" t="s" s="37">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="Q30" s="39"/>
       <c r="R30" s="37"/>
@@ -3835,10 +3846,10 @@
         <v>26</v>
       </c>
       <c r="D31" t="s" s="31">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="E31" t="s" s="32">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F31" s="33">
         <v>44984</v>
@@ -3847,10 +3858,10 @@
         <v>1.680555555555556</v>
       </c>
       <c r="H31" t="s" s="44">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="I31" t="s" s="43">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="J31" t="s" s="37">
         <v>31</v>
@@ -3863,13 +3874,13 @@
         <v>31</v>
       </c>
       <c r="N31" t="s" s="43">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="O31" t="s" s="37">
         <v>47</v>
       </c>
       <c r="P31" t="s" s="37">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="Q31" s="39"/>
       <c r="R31" s="37"/>
@@ -3889,10 +3900,10 @@
         <v>26</v>
       </c>
       <c r="D32" t="s" s="31">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E32" t="s" s="32">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F32" s="33">
         <v>44984</v>
@@ -3901,10 +3912,10 @@
         <v>1.694444444444444</v>
       </c>
       <c r="H32" t="s" s="62">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="I32" t="s" s="43">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="J32" t="s" s="37">
         <v>31</v>
@@ -3917,13 +3928,13 @@
         <v>31</v>
       </c>
       <c r="N32" t="s" s="43">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="O32" t="s" s="37">
         <v>47</v>
       </c>
       <c r="P32" t="s" s="37">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="Q32" s="39"/>
       <c r="R32" s="37"/>
@@ -3943,10 +3954,10 @@
         <v>26</v>
       </c>
       <c r="D33" t="s" s="31">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E33" t="s" s="32">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F33" s="33">
         <v>44984</v>
@@ -3955,10 +3966,10 @@
         <v>1.697916666666667</v>
       </c>
       <c r="H33" t="s" s="63">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="I33" t="s" s="43">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="J33" t="s" s="37">
         <v>31</v>
@@ -3971,13 +3982,13 @@
         <v>31</v>
       </c>
       <c r="N33" t="s" s="43">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="O33" t="s" s="37">
         <v>47</v>
       </c>
       <c r="P33" t="s" s="37">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="Q33" s="39"/>
       <c r="R33" s="37"/>
@@ -3997,10 +4008,10 @@
         <v>26</v>
       </c>
       <c r="D34" t="s" s="31">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="E34" t="s" s="32">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F34" s="33">
         <v>44981</v>
@@ -4009,10 +4020,10 @@
         <v>1.642361111111111</v>
       </c>
       <c r="H34" t="s" s="35">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="I34" t="s" s="43">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="J34" t="s" s="37">
         <v>31</v>
@@ -4025,13 +4036,13 @@
         <v>31</v>
       </c>
       <c r="N34" t="s" s="43">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="O34" t="s" s="37">
         <v>47</v>
       </c>
       <c r="P34" t="s" s="37">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="Q34" s="39"/>
       <c r="R34" s="37"/>
@@ -4051,10 +4062,10 @@
         <v>26</v>
       </c>
       <c r="D35" t="s" s="65">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="E35" t="s" s="66">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="F35" s="51">
         <v>44981</v>
@@ -4063,10 +4074,10 @@
         <v>1.673611111111111</v>
       </c>
       <c r="H35" t="s" s="68">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="I35" t="s" s="69">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="J35" t="s" s="70">
         <v>31</v>
@@ -4079,13 +4090,13 @@
         <v>31</v>
       </c>
       <c r="N35" t="s" s="69">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="O35" t="s" s="70">
         <v>47</v>
       </c>
       <c r="P35" t="s" s="70">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="Q35" s="72"/>
       <c r="R35" s="70"/>
@@ -22736,40 +22747,40 @@
         <v>6</v>
       </c>
       <c r="C1" t="s" s="82">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D1" t="s" s="83">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="E1" s="84"/>
     </row>
     <row r="2" ht="14.25" customHeight="1">
       <c r="A2" t="s" s="85">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B2" t="s" s="86">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C2" t="s" s="87">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="D2" t="s" s="88">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="E2" s="84"/>
     </row>
     <row r="3" ht="14.25" customHeight="1">
       <c r="A3" t="s" s="89">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B3" t="s" s="90">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C3" t="s" s="91">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="D3" t="s" s="92">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E3" s="84"/>
     </row>
@@ -22778,58 +22789,58 @@
         <v>26</v>
       </c>
       <c r="B4" t="s" s="90">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C4" t="s" s="91">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D4" t="s" s="93">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E4" s="84"/>
     </row>
     <row r="5" ht="14.25" customHeight="1">
       <c r="A5" t="s" s="89">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B5" t="s" s="90">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C5" t="s" s="91">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="D5" t="s" s="92">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E5" s="84"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
       <c r="A6" t="s" s="89">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B6" t="s" s="90">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C6" t="s" s="91">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D6" t="s" s="93">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E6" s="84"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
       <c r="A7" t="s" s="94">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B7" t="s" s="95">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C7" t="s" s="96">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="D7" t="s" s="93">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="E7" s="84"/>
     </row>

</xml_diff>

<commit_message>
Risolti errori caso ID 14
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111GESAN000000/GESAN_SRL/WLEXT-RIS/V.2.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111GESAN000000/GESAN_SRL/WLEXT-RIS/V.2.0/report-checklist.xlsx
@@ -52,7 +52,7 @@
     <t>subject_application_vendor: GESAN SRL</t>
   </si>
   <si>
-    <t>subject_application_version: v.2.0</t>
+    <t>subject_application_version: V.2.0</t>
   </si>
   <si>
     <t>ID</t>
@@ -129,10 +129,10 @@
 Il Documento CDA2 Referto Radiologia dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 1" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">225f7ba7c1f23743 </t>
+    <t>af3ef739c0d91a8e</t>
   </si>
   <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.150.4.4.94acb62a90ecf2b5970963e2b6ccecc38052be0abcb8d84f43ef841412b8d449.3e35d8291f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId </t>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.94acb62a90ecf2b5970963e2b6ccecc38052be0abcb8d84f43ef841412b8d449.acaa092191^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>SI</t>
@@ -149,10 +149,10 @@
 Il Documento CDA2 Referto Radiologia dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 2" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">3a6a8847209d21db </t>
+    <t>85574c797e25b6b2</t>
   </si>
   <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.150.4.4.e1419bb55c3a28ea90fec660fd9c487856dba78a3be8356b7ac8788f8cefc5e6.8533ccd671^^^^urn:ihe:iti:xdw:2013:workflowInstanceId </t>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.e1419bb55c3a28ea90fec660fd9c487856dba78a3be8356b7ac8788f8cefc5e6.f0714a35aa^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT3</t>
@@ -163,10 +163,10 @@
 Il Documento CDA2 Referto Radiologia dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 3" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>e119df24bb944ac7</t>
+    <t>f927f9294ef77277</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.7e3a302338821f54720cdcaba959a2d45529ae4de12f5dbf2ab807a409540e19.a0b615ba0d^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.7e3a302338821f54720cdcaba959a2d45529ae4de12f5dbf2ab807a409540e19.52cba350b4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_CDA2_RAD_CT4</t>
@@ -177,10 +177,10 @@
 Il Documento CDA2 Referto Radiologia dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 4" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t xml:space="preserve">3812f577550378e4 </t>
+    <t xml:space="preserve">2964dcfd215876d2 </t>
   </si>
   <si>
-    <t xml:space="preserve">2.16.840.1.113883.2.9.2.150.4.4.674a5c9463de6e1664dc42fbb6927dc235b0571732d102dbc042ffd2b2257e42.349db71e07^^^^urn:ihe:iti:xdw:2013:workflowInstanceId </t>
+    <t xml:space="preserve">2.16.840.1.113883.2.9.2.150.4.4.674a5c9463de6e1664dc42fbb6927dc235b0571732d102dbc042ffd2b2257e42.193395f6b5^^^^urn:ihe:iti:xdw:2013:workflowInstanceId </t>
   </si>
   <si>
     <t>VALIDAZIONE_TOKEN_JWT_RAD_KO</t>
@@ -766,7 +766,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -944,6 +944,21 @@
         <color indexed="8"/>
       </left>
       <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="medium">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
         <color indexed="10"/>
       </right>
       <top style="medium">
@@ -1009,7 +1024,7 @@
       <top style="thin">
         <color indexed="10"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="8"/>
       </bottom>
       <diagonal/>
@@ -1021,10 +1036,10 @@
       <right style="thin">
         <color indexed="8"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="8"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="8"/>
       </bottom>
       <diagonal/>
@@ -1032,6 +1047,21 @@
     <border>
       <left style="thin">
         <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="10"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="10"/>
       </left>
       <right style="thin">
         <color indexed="8"/>
@@ -1067,7 +1097,7 @@
         <color indexed="8"/>
       </right>
       <top style="thin">
-        <color indexed="8"/>
+        <color indexed="10"/>
       </top>
       <bottom style="medium">
         <color indexed="8"/>
@@ -1098,21 +1128,6 @@
       </right>
       <top style="medium">
         <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
       </top>
       <bottom style="thin">
         <color indexed="8"/>
@@ -1215,7 +1230,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -1318,17 +1333,17 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="59" fontId="0" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="60" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="60" fontId="0" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1339,112 +1354,136 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="59" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="59" fontId="0" fillId="2" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="60" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="59" fontId="0" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="2" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="60" fontId="0" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="59" fontId="0" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="59" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="2" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="60" fontId="0" fillId="2" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="60" fontId="0" fillId="2" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="60" fontId="0" fillId="2" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1471,25 +1510,25 @@
     <xf numFmtId="49" fontId="3" fillId="3" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="25" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="26" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="26" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1498,13 +1537,13 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="28" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="28" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="28" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1513,7 +1552,7 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="30" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -2909,10 +2948,10 @@
         <v>29</v>
       </c>
       <c r="F10" s="34">
-        <v>44980</v>
+        <v>45016</v>
       </c>
       <c r="G10" s="35">
-        <v>1.631944444444444</v>
+        <v>1.420138888888889</v>
       </c>
       <c r="H10" t="s" s="36">
         <v>30</v>
@@ -2952,16 +2991,16 @@
       <c r="E11" t="s" s="33">
         <v>35</v>
       </c>
-      <c r="F11" s="34">
-        <v>44980</v>
+      <c r="F11" s="43">
+        <v>45016</v>
       </c>
       <c r="G11" s="35">
-        <v>1.694444444444444</v>
-      </c>
-      <c r="H11" t="s" s="43">
+        <v>1.421527777777778</v>
+      </c>
+      <c r="H11" t="s" s="44">
         <v>36</v>
       </c>
-      <c r="I11" t="s" s="44">
+      <c r="I11" t="s" s="45">
         <v>37</v>
       </c>
       <c r="J11" t="s" s="38">
@@ -2996,16 +3035,16 @@
       <c r="E12" t="s" s="33">
         <v>39</v>
       </c>
-      <c r="F12" s="34">
-        <v>45006</v>
+      <c r="F12" s="43">
+        <v>45016</v>
       </c>
       <c r="G12" s="35">
-        <v>1.40625</v>
-      </c>
-      <c r="H12" t="s" s="45">
+        <v>1.422222222222222</v>
+      </c>
+      <c r="H12" t="s" s="46">
         <v>40</v>
       </c>
-      <c r="I12" t="s" s="44">
+      <c r="I12" t="s" s="47">
         <v>41</v>
       </c>
       <c r="J12" t="s" s="38">
@@ -3040,16 +3079,16 @@
       <c r="E13" t="s" s="33">
         <v>43</v>
       </c>
-      <c r="F13" s="34">
-        <v>44984</v>
-      </c>
-      <c r="G13" s="35">
-        <v>1.509722222222222</v>
-      </c>
-      <c r="H13" t="s" s="46">
+      <c r="F13" s="48">
+        <v>45015</v>
+      </c>
+      <c r="G13" s="49">
+        <v>1.420138888888889</v>
+      </c>
+      <c r="H13" t="s" s="50">
         <v>44</v>
       </c>
-      <c r="I13" t="s" s="47">
+      <c r="I13" t="s" s="51">
         <v>45</v>
       </c>
       <c r="J13" t="s" s="38">
@@ -3081,17 +3120,17 @@
       <c r="D14" t="s" s="32">
         <v>46</v>
       </c>
-      <c r="E14" t="s" s="48">
+      <c r="E14" t="s" s="52">
         <v>47</v>
       </c>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="34"/>
+      <c r="F14" s="53"/>
+      <c r="G14" s="48"/>
+      <c r="H14" s="53"/>
+      <c r="I14" s="53"/>
       <c r="J14" t="s" s="38">
         <v>48</v>
       </c>
-      <c r="K14" t="s" s="49">
+      <c r="K14" t="s" s="54">
         <v>49</v>
       </c>
       <c r="L14" s="40"/>
@@ -3119,38 +3158,38 @@
       <c r="D15" t="s" s="32">
         <v>51</v>
       </c>
-      <c r="E15" t="s" s="48">
+      <c r="E15" t="s" s="52">
         <v>52</v>
       </c>
-      <c r="F15" s="34">
+      <c r="F15" s="53">
         <v>44987</v>
       </c>
-      <c r="G15" t="s" s="50">
+      <c r="G15" t="s" s="55">
         <v>53</v>
       </c>
-      <c r="H15" t="s" s="51">
+      <c r="H15" t="s" s="56">
         <v>54</v>
       </c>
-      <c r="I15" t="s" s="51">
+      <c r="I15" t="s" s="56">
         <v>55</v>
       </c>
       <c r="J15" t="s" s="38">
         <v>32</v>
       </c>
-      <c r="K15" s="52"/>
+      <c r="K15" s="57"/>
       <c r="L15" t="s" s="38">
         <v>32</v>
       </c>
       <c r="M15" t="s" s="38">
         <v>48</v>
       </c>
-      <c r="N15" t="s" s="49">
+      <c r="N15" t="s" s="54">
         <v>56</v>
       </c>
       <c r="O15" t="s" s="38">
         <v>32</v>
       </c>
-      <c r="P15" t="s" s="49">
+      <c r="P15" t="s" s="54">
         <v>57</v>
       </c>
       <c r="Q15" s="40"/>
@@ -3176,21 +3215,21 @@
       <c r="E16" t="s" s="33">
         <v>59</v>
       </c>
-      <c r="F16" s="53">
+      <c r="F16" s="34">
         <v>44987</v>
       </c>
-      <c r="G16" t="s" s="51">
+      <c r="G16" t="s" s="56">
         <v>60</v>
       </c>
-      <c r="H16" s="54"/>
-      <c r="I16" s="54"/>
+      <c r="H16" s="43"/>
+      <c r="I16" s="43"/>
       <c r="J16" s="40"/>
       <c r="K16" s="39"/>
       <c r="L16" s="40"/>
       <c r="M16" s="40"/>
-      <c r="N16" s="52"/>
+      <c r="N16" s="57"/>
       <c r="O16" s="40"/>
-      <c r="P16" t="s" s="55">
+      <c r="P16" t="s" s="58">
         <v>61</v>
       </c>
       <c r="Q16" s="40"/>
@@ -3215,13 +3254,13 @@
       <c r="D17" t="s" s="32">
         <v>62</v>
       </c>
-      <c r="E17" t="s" s="56">
+      <c r="E17" t="s" s="59">
         <v>63</v>
       </c>
-      <c r="F17" s="57"/>
-      <c r="G17" s="57"/>
-      <c r="H17" s="57"/>
-      <c r="I17" s="58"/>
+      <c r="F17" s="60"/>
+      <c r="G17" s="60"/>
+      <c r="H17" s="60"/>
+      <c r="I17" s="61"/>
       <c r="J17" t="s" s="38">
         <v>48</v>
       </c>
@@ -3256,10 +3295,10 @@
       <c r="E18" t="s" s="33">
         <v>66</v>
       </c>
-      <c r="F18" s="34"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="53"/>
-      <c r="I18" s="53"/>
+      <c r="F18" s="53"/>
+      <c r="G18" s="53"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="34"/>
       <c r="J18" t="s" s="38">
         <v>48</v>
       </c>
@@ -3268,7 +3307,7 @@
       </c>
       <c r="L18" s="40"/>
       <c r="M18" s="40"/>
-      <c r="N18" s="59"/>
+      <c r="N18" s="62"/>
       <c r="O18" s="40"/>
       <c r="P18" s="39"/>
       <c r="Q18" s="40"/>
@@ -3294,7 +3333,7 @@
       <c r="E19" t="s" s="33">
         <v>69</v>
       </c>
-      <c r="F19" s="34">
+      <c r="F19" s="53">
         <v>44981</v>
       </c>
       <c r="G19" s="35">
@@ -3313,10 +3352,10 @@
       <c r="L19" t="s" s="38">
         <v>32</v>
       </c>
-      <c r="M19" t="s" s="60">
+      <c r="M19" t="s" s="63">
         <v>48</v>
       </c>
-      <c r="N19" t="s" s="37">
+      <c r="N19" t="s" s="64">
         <v>72</v>
       </c>
       <c r="O19" t="s" s="38">
@@ -3348,16 +3387,16 @@
       <c r="E20" t="s" s="33">
         <v>75</v>
       </c>
-      <c r="F20" s="34">
+      <c r="F20" s="53">
         <v>44981</v>
       </c>
       <c r="G20" s="35">
         <v>1.6125</v>
       </c>
-      <c r="H20" t="s" s="46">
+      <c r="H20" t="s" s="65">
         <v>76</v>
       </c>
-      <c r="I20" t="s" s="47">
+      <c r="I20" t="s" s="66">
         <v>77</v>
       </c>
       <c r="J20" t="s" s="38">
@@ -3367,10 +3406,10 @@
       <c r="L20" t="s" s="38">
         <v>32</v>
       </c>
-      <c r="M20" t="s" s="60">
+      <c r="M20" t="s" s="63">
         <v>32</v>
       </c>
-      <c r="N20" t="s" s="47">
+      <c r="N20" t="s" s="67">
         <v>78</v>
       </c>
       <c r="O20" t="s" s="38">
@@ -3402,10 +3441,10 @@
       <c r="E21" t="s" s="33">
         <v>81</v>
       </c>
-      <c r="F21" s="34"/>
-      <c r="G21" s="34"/>
-      <c r="H21" s="34"/>
-      <c r="I21" s="34"/>
+      <c r="F21" s="53"/>
+      <c r="G21" s="53"/>
+      <c r="H21" s="53"/>
+      <c r="I21" s="53"/>
       <c r="J21" t="s" s="38">
         <v>48</v>
       </c>
@@ -3440,10 +3479,10 @@
       <c r="E22" t="s" s="33">
         <v>83</v>
       </c>
-      <c r="F22" s="34"/>
-      <c r="G22" s="34"/>
-      <c r="H22" s="53"/>
-      <c r="I22" s="53"/>
+      <c r="F22" s="53"/>
+      <c r="G22" s="53"/>
+      <c r="H22" s="34"/>
+      <c r="I22" s="34"/>
       <c r="J22" t="s" s="38">
         <v>48</v>
       </c>
@@ -3452,7 +3491,7 @@
       </c>
       <c r="L22" s="40"/>
       <c r="M22" s="40"/>
-      <c r="N22" s="59"/>
+      <c r="N22" s="62"/>
       <c r="O22" s="40"/>
       <c r="P22" s="39"/>
       <c r="Q22" s="40"/>
@@ -3478,16 +3517,16 @@
       <c r="E23" t="s" s="33">
         <v>85</v>
       </c>
-      <c r="F23" s="34">
+      <c r="F23" s="53">
         <v>44981</v>
       </c>
       <c r="G23" s="35">
         <v>1.665277777777778</v>
       </c>
-      <c r="H23" t="s" s="61">
+      <c r="H23" t="s" s="68">
         <v>86</v>
       </c>
-      <c r="I23" t="s" s="62">
+      <c r="I23" t="s" s="51">
         <v>87</v>
       </c>
       <c r="J23" t="s" s="38">
@@ -3497,10 +3536,10 @@
       <c r="L23" t="s" s="38">
         <v>32</v>
       </c>
-      <c r="M23" t="s" s="60">
+      <c r="M23" t="s" s="63">
         <v>32</v>
       </c>
-      <c r="N23" t="s" s="62">
+      <c r="N23" t="s" s="69">
         <v>88</v>
       </c>
       <c r="O23" t="s" s="38">
@@ -3532,10 +3571,10 @@
       <c r="E24" t="s" s="33">
         <v>91</v>
       </c>
-      <c r="F24" s="34"/>
-      <c r="G24" s="34"/>
-      <c r="H24" s="34"/>
-      <c r="I24" s="34"/>
+      <c r="F24" s="53"/>
+      <c r="G24" s="53"/>
+      <c r="H24" s="53"/>
+      <c r="I24" s="53"/>
       <c r="J24" t="s" s="38">
         <v>48</v>
       </c>
@@ -3570,10 +3609,10 @@
       <c r="E25" t="s" s="33">
         <v>94</v>
       </c>
-      <c r="F25" s="34"/>
-      <c r="G25" s="34"/>
-      <c r="H25" s="53"/>
-      <c r="I25" s="53"/>
+      <c r="F25" s="53"/>
+      <c r="G25" s="53"/>
+      <c r="H25" s="34"/>
+      <c r="I25" s="34"/>
       <c r="J25" t="s" s="38">
         <v>48</v>
       </c>
@@ -3582,7 +3621,7 @@
       </c>
       <c r="L25" s="40"/>
       <c r="M25" s="40"/>
-      <c r="N25" s="59"/>
+      <c r="N25" s="62"/>
       <c r="O25" s="40"/>
       <c r="P25" s="39"/>
       <c r="Q25" s="40"/>
@@ -3608,16 +3647,16 @@
       <c r="E26" t="s" s="33">
         <v>96</v>
       </c>
-      <c r="F26" s="34">
+      <c r="F26" s="53">
         <v>44981</v>
       </c>
       <c r="G26" s="35">
         <v>1.613194444444444</v>
       </c>
-      <c r="H26" t="s" s="61">
+      <c r="H26" t="s" s="68">
         <v>97</v>
       </c>
-      <c r="I26" t="s" s="62">
+      <c r="I26" t="s" s="51">
         <v>98</v>
       </c>
       <c r="J26" t="s" s="38">
@@ -3627,10 +3666,10 @@
       <c r="L26" t="s" s="38">
         <v>32</v>
       </c>
-      <c r="M26" t="s" s="60">
+      <c r="M26" t="s" s="63">
         <v>32</v>
       </c>
-      <c r="N26" t="s" s="62">
+      <c r="N26" t="s" s="69">
         <v>99</v>
       </c>
       <c r="O26" t="s" s="38">
@@ -3662,10 +3701,10 @@
       <c r="E27" t="s" s="33">
         <v>102</v>
       </c>
-      <c r="F27" s="34"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="53"/>
-      <c r="I27" s="53"/>
+      <c r="F27" s="53"/>
+      <c r="G27" s="53"/>
+      <c r="H27" s="34"/>
+      <c r="I27" s="34"/>
       <c r="J27" t="s" s="38">
         <v>48</v>
       </c>
@@ -3674,7 +3713,7 @@
       </c>
       <c r="L27" s="40"/>
       <c r="M27" s="40"/>
-      <c r="N27" s="59"/>
+      <c r="N27" s="62"/>
       <c r="O27" s="40"/>
       <c r="P27" s="39"/>
       <c r="Q27" s="40"/>
@@ -3700,7 +3739,7 @@
       <c r="E28" t="s" s="33">
         <v>105</v>
       </c>
-      <c r="F28" s="34">
+      <c r="F28" s="53">
         <v>44981</v>
       </c>
       <c r="G28" s="35">
@@ -3719,10 +3758,10 @@
       <c r="L28" t="s" s="38">
         <v>32</v>
       </c>
-      <c r="M28" t="s" s="60">
+      <c r="M28" t="s" s="63">
         <v>32</v>
       </c>
-      <c r="N28" t="s" s="37">
+      <c r="N28" t="s" s="64">
         <v>108</v>
       </c>
       <c r="O28" t="s" s="38">
@@ -3754,16 +3793,16 @@
       <c r="E29" t="s" s="33">
         <v>111</v>
       </c>
-      <c r="F29" s="34">
+      <c r="F29" s="53">
         <v>44981</v>
       </c>
       <c r="G29" s="35">
         <v>1.634027777777778</v>
       </c>
-      <c r="H29" t="s" s="43">
+      <c r="H29" t="s" s="44">
         <v>112</v>
       </c>
-      <c r="I29" t="s" s="44">
+      <c r="I29" t="s" s="45">
         <v>113</v>
       </c>
       <c r="J29" t="s" s="38">
@@ -3773,10 +3812,10 @@
       <c r="L29" t="s" s="38">
         <v>32</v>
       </c>
-      <c r="M29" t="s" s="60">
+      <c r="M29" t="s" s="63">
         <v>32</v>
       </c>
-      <c r="N29" t="s" s="44">
+      <c r="N29" t="s" s="70">
         <v>114</v>
       </c>
       <c r="O29" t="s" s="38">
@@ -3808,16 +3847,16 @@
       <c r="E30" t="s" s="33">
         <v>117</v>
       </c>
-      <c r="F30" s="34">
+      <c r="F30" s="53">
         <v>44984</v>
       </c>
       <c r="G30" s="35">
         <v>1.517361111111111</v>
       </c>
-      <c r="H30" t="s" s="43">
+      <c r="H30" t="s" s="44">
         <v>118</v>
       </c>
-      <c r="I30" t="s" s="44">
+      <c r="I30" t="s" s="45">
         <v>119</v>
       </c>
       <c r="J30" t="s" s="38">
@@ -3827,10 +3866,10 @@
       <c r="L30" t="s" s="38">
         <v>32</v>
       </c>
-      <c r="M30" t="s" s="60">
+      <c r="M30" t="s" s="63">
         <v>32</v>
       </c>
-      <c r="N30" t="s" s="44">
+      <c r="N30" t="s" s="70">
         <v>120</v>
       </c>
       <c r="O30" t="s" s="38">
@@ -3862,16 +3901,16 @@
       <c r="E31" t="s" s="33">
         <v>123</v>
       </c>
-      <c r="F31" s="34">
+      <c r="F31" s="53">
         <v>44984</v>
       </c>
       <c r="G31" s="35">
         <v>1.680555555555556</v>
       </c>
-      <c r="H31" t="s" s="46">
+      <c r="H31" t="s" s="65">
         <v>124</v>
       </c>
-      <c r="I31" t="s" s="44">
+      <c r="I31" t="s" s="45">
         <v>125</v>
       </c>
       <c r="J31" t="s" s="38">
@@ -3881,10 +3920,10 @@
       <c r="L31" t="s" s="38">
         <v>32</v>
       </c>
-      <c r="M31" t="s" s="60">
+      <c r="M31" t="s" s="63">
         <v>32</v>
       </c>
-      <c r="N31" t="s" s="44">
+      <c r="N31" t="s" s="70">
         <v>126</v>
       </c>
       <c r="O31" t="s" s="38">
@@ -3916,16 +3955,16 @@
       <c r="E32" t="s" s="33">
         <v>129</v>
       </c>
-      <c r="F32" s="34">
+      <c r="F32" s="53">
         <v>44984</v>
       </c>
-      <c r="G32" s="63">
+      <c r="G32" s="71">
         <v>1.694444444444444</v>
       </c>
-      <c r="H32" t="s" s="64">
+      <c r="H32" t="s" s="72">
         <v>130</v>
       </c>
-      <c r="I32" t="s" s="44">
+      <c r="I32" t="s" s="45">
         <v>131</v>
       </c>
       <c r="J32" t="s" s="38">
@@ -3935,10 +3974,10 @@
       <c r="L32" t="s" s="38">
         <v>32</v>
       </c>
-      <c r="M32" t="s" s="60">
+      <c r="M32" t="s" s="63">
         <v>32</v>
       </c>
-      <c r="N32" t="s" s="44">
+      <c r="N32" t="s" s="70">
         <v>132</v>
       </c>
       <c r="O32" t="s" s="38">
@@ -3970,16 +4009,16 @@
       <c r="E33" t="s" s="33">
         <v>135</v>
       </c>
-      <c r="F33" s="34">
+      <c r="F33" s="53">
         <v>44984</v>
       </c>
-      <c r="G33" s="63">
+      <c r="G33" s="71">
         <v>1.697916666666667</v>
       </c>
-      <c r="H33" t="s" s="65">
+      <c r="H33" t="s" s="73">
         <v>136</v>
       </c>
-      <c r="I33" t="s" s="44">
+      <c r="I33" t="s" s="45">
         <v>137</v>
       </c>
       <c r="J33" t="s" s="38">
@@ -3989,10 +4028,10 @@
       <c r="L33" t="s" s="38">
         <v>32</v>
       </c>
-      <c r="M33" t="s" s="60">
+      <c r="M33" t="s" s="63">
         <v>32</v>
       </c>
-      <c r="N33" t="s" s="44">
+      <c r="N33" t="s" s="70">
         <v>138</v>
       </c>
       <c r="O33" t="s" s="38">
@@ -4024,7 +4063,7 @@
       <c r="E34" t="s" s="33">
         <v>141</v>
       </c>
-      <c r="F34" s="34">
+      <c r="F34" s="53">
         <v>44981</v>
       </c>
       <c r="G34" s="35">
@@ -4033,7 +4072,7 @@
       <c r="H34" t="s" s="36">
         <v>142</v>
       </c>
-      <c r="I34" t="s" s="44">
+      <c r="I34" t="s" s="45">
         <v>143</v>
       </c>
       <c r="J34" t="s" s="38">
@@ -4043,10 +4082,10 @@
       <c r="L34" t="s" s="38">
         <v>32</v>
       </c>
-      <c r="M34" t="s" s="60">
+      <c r="M34" t="s" s="63">
         <v>32</v>
       </c>
-      <c r="N34" t="s" s="44">
+      <c r="N34" t="s" s="70">
         <v>144</v>
       </c>
       <c r="O34" t="s" s="38">
@@ -4063,56 +4102,56 @@
       </c>
     </row>
     <row r="35" ht="222.05" customHeight="1">
-      <c r="A35" s="66">
+      <c r="A35" s="74">
         <v>93</v>
       </c>
-      <c r="B35" t="s" s="67">
+      <c r="B35" t="s" s="75">
         <v>26</v>
       </c>
-      <c r="C35" t="s" s="67">
+      <c r="C35" t="s" s="75">
         <v>27</v>
       </c>
-      <c r="D35" t="s" s="67">
+      <c r="D35" t="s" s="75">
         <v>146</v>
       </c>
-      <c r="E35" t="s" s="68">
+      <c r="E35" t="s" s="76">
         <v>147</v>
       </c>
-      <c r="F35" s="53">
+      <c r="F35" s="34">
         <v>44981</v>
       </c>
-      <c r="G35" s="69">
+      <c r="G35" s="77">
         <v>1.673611111111111</v>
       </c>
-      <c r="H35" t="s" s="70">
+      <c r="H35" t="s" s="78">
         <v>148</v>
       </c>
-      <c r="I35" t="s" s="71">
+      <c r="I35" t="s" s="47">
         <v>149</v>
       </c>
-      <c r="J35" t="s" s="72">
+      <c r="J35" t="s" s="79">
         <v>32</v>
       </c>
-      <c r="K35" s="59"/>
-      <c r="L35" t="s" s="72">
+      <c r="K35" s="62"/>
+      <c r="L35" t="s" s="79">
         <v>32</v>
       </c>
-      <c r="M35" t="s" s="73">
+      <c r="M35" t="s" s="80">
         <v>32</v>
       </c>
-      <c r="N35" t="s" s="71">
+      <c r="N35" t="s" s="81">
         <v>150</v>
       </c>
-      <c r="O35" t="s" s="72">
+      <c r="O35" t="s" s="79">
         <v>48</v>
       </c>
-      <c r="P35" t="s" s="72">
+      <c r="P35" t="s" s="79">
         <v>151</v>
       </c>
-      <c r="Q35" s="74"/>
-      <c r="R35" s="72"/>
-      <c r="S35" s="75"/>
-      <c r="T35" t="s" s="76">
+      <c r="Q35" s="82"/>
+      <c r="R35" s="79"/>
+      <c r="S35" s="83"/>
+      <c r="T35" t="s" s="84">
         <v>50</v>
       </c>
     </row>
@@ -4122,21 +4161,21 @@
       <c r="C36" s="20"/>
       <c r="D36" s="20"/>
       <c r="E36" s="20"/>
-      <c r="F36" s="77"/>
-      <c r="G36" s="77"/>
-      <c r="H36" s="77"/>
-      <c r="I36" s="77"/>
-      <c r="J36" s="78"/>
-      <c r="K36" s="78"/>
-      <c r="L36" s="79"/>
-      <c r="M36" s="79"/>
-      <c r="N36" s="78"/>
-      <c r="O36" s="79"/>
-      <c r="P36" s="78"/>
-      <c r="Q36" s="78"/>
-      <c r="R36" s="80"/>
-      <c r="S36" s="81"/>
-      <c r="T36" s="78"/>
+      <c r="F36" s="85"/>
+      <c r="G36" s="85"/>
+      <c r="H36" s="85"/>
+      <c r="I36" s="85"/>
+      <c r="J36" s="86"/>
+      <c r="K36" s="86"/>
+      <c r="L36" s="87"/>
+      <c r="M36" s="87"/>
+      <c r="N36" s="86"/>
+      <c r="O36" s="87"/>
+      <c r="P36" s="86"/>
+      <c r="Q36" s="86"/>
+      <c r="R36" s="88"/>
+      <c r="S36" s="89"/>
+      <c r="T36" s="86"/>
     </row>
     <row r="37" ht="13.55" customHeight="1">
       <c r="A37" s="3"/>
@@ -22742,123 +22781,123 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="16" style="82" customWidth="1"/>
-    <col min="2" max="2" width="23.8516" style="82" customWidth="1"/>
-    <col min="3" max="3" width="18.8516" style="82" customWidth="1"/>
-    <col min="4" max="4" width="58.5" style="82" customWidth="1"/>
-    <col min="5" max="5" width="8.85156" style="82" customWidth="1"/>
-    <col min="6" max="16384" width="14.5" style="82" customWidth="1"/>
+    <col min="1" max="1" width="16" style="90" customWidth="1"/>
+    <col min="2" max="2" width="23.8516" style="90" customWidth="1"/>
+    <col min="3" max="3" width="18.8516" style="90" customWidth="1"/>
+    <col min="4" max="4" width="58.5" style="90" customWidth="1"/>
+    <col min="5" max="5" width="8.85156" style="90" customWidth="1"/>
+    <col min="6" max="16384" width="14.5" style="90" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="14.25" customHeight="1">
-      <c r="A1" t="s" s="83">
+      <c r="A1" t="s" s="91">
         <v>8</v>
       </c>
-      <c r="B1" t="s" s="84">
+      <c r="B1" t="s" s="92">
         <v>7</v>
       </c>
-      <c r="C1" t="s" s="84">
+      <c r="C1" t="s" s="92">
         <v>152</v>
       </c>
-      <c r="D1" t="s" s="85">
+      <c r="D1" t="s" s="93">
         <v>153</v>
       </c>
-      <c r="E1" s="86"/>
+      <c r="E1" s="94"/>
     </row>
     <row r="2" ht="14.25" customHeight="1">
-      <c r="A2" t="s" s="87">
+      <c r="A2" t="s" s="95">
         <v>154</v>
       </c>
-      <c r="B2" t="s" s="88">
+      <c r="B2" t="s" s="96">
         <v>155</v>
       </c>
-      <c r="C2" t="s" s="89">
+      <c r="C2" t="s" s="97">
         <v>156</v>
       </c>
-      <c r="D2" t="s" s="90">
+      <c r="D2" t="s" s="98">
         <v>157</v>
       </c>
-      <c r="E2" s="86"/>
+      <c r="E2" s="94"/>
     </row>
     <row r="3" ht="14.25" customHeight="1">
-      <c r="A3" t="s" s="91">
+      <c r="A3" t="s" s="99">
         <v>158</v>
       </c>
-      <c r="B3" t="s" s="92">
+      <c r="B3" t="s" s="100">
         <v>155</v>
       </c>
-      <c r="C3" t="s" s="93">
+      <c r="C3" t="s" s="101">
         <v>159</v>
       </c>
-      <c r="D3" t="s" s="94">
+      <c r="D3" t="s" s="102">
         <v>160</v>
       </c>
-      <c r="E3" s="86"/>
+      <c r="E3" s="94"/>
     </row>
     <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" t="s" s="91">
+      <c r="A4" t="s" s="99">
         <v>27</v>
       </c>
-      <c r="B4" t="s" s="92">
+      <c r="B4" t="s" s="100">
         <v>155</v>
       </c>
-      <c r="C4" t="s" s="93">
+      <c r="C4" t="s" s="101">
         <v>161</v>
       </c>
-      <c r="D4" t="s" s="95">
+      <c r="D4" t="s" s="103">
         <v>162</v>
       </c>
-      <c r="E4" s="86"/>
+      <c r="E4" s="94"/>
     </row>
     <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" t="s" s="91">
+      <c r="A5" t="s" s="99">
         <v>163</v>
       </c>
-      <c r="B5" t="s" s="92">
+      <c r="B5" t="s" s="100">
         <v>155</v>
       </c>
-      <c r="C5" t="s" s="93">
+      <c r="C5" t="s" s="101">
         <v>164</v>
       </c>
-      <c r="D5" t="s" s="94">
+      <c r="D5" t="s" s="102">
         <v>165</v>
       </c>
-      <c r="E5" s="86"/>
+      <c r="E5" s="94"/>
     </row>
     <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" t="s" s="91">
+      <c r="A6" t="s" s="99">
         <v>166</v>
       </c>
-      <c r="B6" t="s" s="92">
+      <c r="B6" t="s" s="100">
         <v>155</v>
       </c>
-      <c r="C6" t="s" s="93">
+      <c r="C6" t="s" s="101">
         <v>167</v>
       </c>
-      <c r="D6" t="s" s="95">
+      <c r="D6" t="s" s="103">
         <v>168</v>
       </c>
-      <c r="E6" s="86"/>
+      <c r="E6" s="94"/>
     </row>
     <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" t="s" s="96">
+      <c r="A7" t="s" s="104">
         <v>169</v>
       </c>
-      <c r="B7" t="s" s="97">
+      <c r="B7" t="s" s="105">
         <v>155</v>
       </c>
-      <c r="C7" t="s" s="98">
+      <c r="C7" t="s" s="106">
         <v>170</v>
       </c>
-      <c r="D7" t="s" s="95">
+      <c r="D7" t="s" s="103">
         <v>171</v>
       </c>
-      <c r="E7" s="86"/>
+      <c r="E7" s="94"/>
     </row>
     <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" s="99"/>
-      <c r="B8" s="99"/>
-      <c r="C8" s="99"/>
+      <c r="A8" s="107"/>
+      <c r="B8" s="107"/>
+      <c r="C8" s="107"/>
       <c r="D8" s="20"/>
       <c r="E8" s="3"/>
     </row>

</xml_diff>

<commit_message>
Corretti errori casi test id 11, 14
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111GESAN000000/GESAN_SRL/WLEXT-RIS/V.2.0/report-checklist.xlsx
+++ b/GATEWAY/A1#111GESAN000000/GESAN_SRL/WLEXT-RIS/V.2.0/report-checklist.xlsx
@@ -129,10 +129,10 @@
 Il Documento CDA2 Referto Radiologia dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 1" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>211fc56f3d91adfb</t>
+    <t>6796e42e492b1d90</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.94acb62a90ecf2b5970963e2b6ccecc38052be0abcb8d84f43ef841412b8d449.466167137e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.94acb62a90ecf2b5970963e2b6ccecc38052be0abcb8d84f43ef841412b8d449.82c68babf6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>SI</t>
@@ -177,10 +177,10 @@
 Il Documento CDA2 Referto Radiologia dovrà essere composto in moda da risultare valido dal punto di vista sintattico, semantico, terminologico. I dati utilizzati per comporre il CDA2 dovranno essere conformi alle section e le entry secondo quanto espresso dalla sezione "CASO DI TEST 4" riportata nei documenti "casi di test RAD" e "CDA2_Referto_di_Radiologia_OK" presenti al path https://github.com/ministero-salute/it-fse-accreditamento.</t>
   </si>
   <si>
-    <t>2187e5ff744f75ea</t>
+    <t>c4b5aecafad85263</t>
   </si>
   <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.674a5c9463de6e1664dc42fbb6927dc235b0571732d102dbc042ffd2b2257e42.a519f57962^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.674a5c9463de6e1664dc42fbb6927dc235b0571732d102dbc042ffd2b2257e42.548228583e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
     <t>VALIDAZIONE_TOKEN_JWT_RAD_KO</t>
@@ -2948,10 +2948,10 @@
         <v>29</v>
       </c>
       <c r="F10" s="34">
-        <v>45030</v>
+        <v>45035</v>
       </c>
       <c r="G10" s="35">
-        <v>1.742361111111111</v>
+        <v>1.408333333333333</v>
       </c>
       <c r="H10" t="s" s="36">
         <v>30</v>
@@ -3080,10 +3080,10 @@
         <v>43</v>
       </c>
       <c r="F13" s="47">
-        <v>45030</v>
+        <v>45035</v>
       </c>
       <c r="G13" s="48">
-        <v>1.744444444444444</v>
+        <v>1.410416666666667</v>
       </c>
       <c r="H13" t="s" s="49">
         <v>44</v>

</xml_diff>